<commit_message>
changed demographics column names
</commit_message>
<xml_diff>
--- a/Updating Shiny Data/ACS Variables.xlsx
+++ b/Updating Shiny Data/ACS Variables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valans/Documents/WORK/UMASS/SEIGMA/R/New Data Cleaning FIles/APIs/Census API/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valans/SEIGMA/Updating Shiny Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DDDCE8-1C6D-1D44-B85E-210DBF55595C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7951B845-B5FB-3045-9BBC-AD66E4EDCD18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3820" yWindow="460" windowWidth="21080" windowHeight="14320" xr2:uid="{7F4859F1-A9CE-0C44-A2BA-0CFBFFD44F8C}"/>
   </bookViews>
@@ -165,12 +165,6 @@
     <t>Margin_Error_Hawaiian_and_Other_Pacific_Islander_Pct</t>
   </si>
   <si>
-    <t>Others_Pct</t>
-  </si>
-  <si>
-    <t>Margin_Error_Others_Pct</t>
-  </si>
-  <si>
     <t>Hispanic_Pct</t>
   </si>
   <si>
@@ -940,6 +934,12 @@
   </si>
   <si>
     <t>Rent.Margin.of.Error.2017.Dollar</t>
+  </si>
+  <si>
+    <t>Other_Pct</t>
+  </si>
+  <si>
+    <t>Margin_Error_Other_Pct</t>
   </si>
 </sst>
 </file>
@@ -1345,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1848B443-3138-894C-9499-8E1786236A09}">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1360,27 +1360,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1388,13 +1388,13 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1402,13 +1402,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1416,13 +1416,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1430,13 +1430,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1444,13 +1444,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1458,13 +1458,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1472,13 +1472,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1486,13 +1486,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1500,13 +1500,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1514,13 +1514,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1528,13 +1528,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1542,13 +1542,13 @@
         <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1556,13 +1556,13 @@
         <v>12</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1570,13 +1570,13 @@
         <v>13</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1584,13 +1584,13 @@
         <v>14</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1598,13 +1598,13 @@
         <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1612,13 +1612,13 @@
         <v>16</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1626,13 +1626,13 @@
         <v>17</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1640,13 +1640,13 @@
         <v>18</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1654,13 +1654,13 @@
         <v>19</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1668,13 +1668,13 @@
         <v>20</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1682,13 +1682,13 @@
         <v>21</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1696,13 +1696,13 @@
         <v>22</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>194</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1710,13 +1710,13 @@
         <v>23</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1724,13 +1724,13 @@
         <v>24</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1738,13 +1738,13 @@
         <v>25</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1752,13 +1752,13 @@
         <v>26</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1766,13 +1766,13 @@
         <v>27</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1780,13 +1780,13 @@
         <v>28</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1794,13 +1794,13 @@
         <v>29</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1808,27 +1808,27 @@
         <v>30</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1836,13 +1836,13 @@
         <v>31</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1850,13 +1850,13 @@
         <v>32</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1864,13 +1864,13 @@
         <v>33</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1878,13 +1878,13 @@
         <v>34</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1892,13 +1892,13 @@
         <v>35</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1906,13 +1906,13 @@
         <v>36</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1920,13 +1920,13 @@
         <v>37</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1934,13 +1934,13 @@
         <v>38</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1948,13 +1948,13 @@
         <v>39</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D43" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1962,97 +1962,97 @@
         <v>40</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D44" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>41</v>
+        <v>298</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D45" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>42</v>
+        <v>299</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C47" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C48" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -2079,373 +2079,373 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2471,65 +2471,65 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2555,109 +2555,109 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -2683,80 +2683,80 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -2787,128 +2787,128 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="85" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -2933,44 +2933,44 @@
   <sheetData>
     <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>253</v>
-      </c>
       <c r="C3" s="9" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -2995,43 +2995,43 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>